<commit_message>
Refactor gantt chart 1
</commit_message>
<xml_diff>
--- a/SE202526/Management/Sprint1/Gantt_Chart_Sprint1.xlsx
+++ b/SE202526/Management/Sprint1/Gantt_Chart_Sprint1.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29328"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E0AA6536-6850-4033-B33C-9A7FDAC1D07F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{F8EE5A57-812B-4DB1-B36A-9A3DB829BC25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1019,7 +1019,7 @@
   <dimension ref="B1:BP30"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="T6" sqref="T6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.21875" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1390,16 +1390,16 @@
         <v>27</v>
       </c>
       <c r="D5" s="7">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E5" s="7">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F5" s="7">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G5" s="7">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="H5" s="4">
         <v>1</v>
@@ -1413,16 +1413,16 @@
         <v>28</v>
       </c>
       <c r="D6" s="7">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E6" s="7">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F6" s="7">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="G6" s="7">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H6" s="4">
         <v>1</v>

</xml_diff>